<commit_message>
done query for leasing system setup
</commit_message>
<xml_diff>
--- a/TMS Database mapping.xlsx
+++ b/TMS Database mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="lists of all tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9719" uniqueCount="2133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9793" uniqueCount="2133">
   <si>
     <t>new TMS</t>
   </si>
@@ -132,277 +132,283 @@
     <t>t_m_s_clients</t>
   </si>
   <si>
+    <t>tenantaccountfile</t>
+  </si>
+  <si>
+    <t>business_units</t>
+  </si>
+  <si>
+    <t>amendparticularsfile</t>
+  </si>
+  <si>
+    <t>chargesfile</t>
+  </si>
+  <si>
+    <t>t_m_s_tenant_types</t>
+  </si>
+  <si>
+    <t>tenanttypefile</t>
+  </si>
+  <si>
+    <t>companies</t>
+  </si>
+  <si>
+    <t>amendpayschedulefile</t>
+  </si>
+  <si>
+    <t>clausesfile</t>
+  </si>
+  <si>
+    <t>t_m_s_business_categories</t>
+  </si>
+  <si>
+    <t>businesscategoryfile</t>
+  </si>
+  <si>
+    <t>amendrentalchargesfile</t>
+  </si>
+  <si>
+    <t>clientofferfile</t>
+  </si>
+  <si>
+    <t>t_m_s_rental_schemes</t>
+  </si>
+  <si>
+    <t>rentalschemefile</t>
+  </si>
+  <si>
+    <t>e_b_m_authorized_signatories</t>
+  </si>
+  <si>
+    <t>approveby</t>
+  </si>
+  <si>
+    <t>clienttypefile</t>
+  </si>
+  <si>
+    <t>t_m_s_charges</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>e_b_m_billing_terms</t>
+  </si>
+  <si>
+    <t>ar1</t>
+  </si>
+  <si>
+    <t>doctypefile</t>
+  </si>
+  <si>
+    <t>e_b_m_event_types</t>
+  </si>
+  <si>
+    <t>ar2</t>
+  </si>
+  <si>
+    <t>documentfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events</t>
+  </si>
+  <si>
+    <t>at_copy</t>
+  </si>
+  <si>
+    <t>epfdoctypefile</t>
+  </si>
+  <si>
+    <t>SYSTEM SETUP - OPERATION</t>
+  </si>
+  <si>
+    <t>t_m_s_preconstruction_requirements</t>
+  </si>
+  <si>
+    <t>preconstructionfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_amendment</t>
+  </si>
+  <si>
+    <t>epftypefile</t>
+  </si>
+  <si>
+    <t>t_m_s_preoperational_requirements</t>
+  </si>
+  <si>
+    <t>preoperationfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_amendment_information</t>
+  </si>
+  <si>
+    <t>aur_sig</t>
+  </si>
+  <si>
+    <t>eventclassfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_epf_information</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>eventfile</t>
+  </si>
+  <si>
+    <t>t_m_s_provisions</t>
+  </si>
+  <si>
+    <t>provisionsfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_ingress_egress</t>
+  </si>
+  <si>
+    <t>bankfile</t>
+  </si>
+  <si>
+    <t>eventperiodcoveredfile</t>
+  </si>
+  <si>
+    <t>t_m_s_meters</t>
+  </si>
+  <si>
+    <t>meterfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_moa_information</t>
+  </si>
+  <si>
+    <t>eventschedulefile</t>
+  </si>
+  <si>
+    <t>t_m_s_operational_hours</t>
+  </si>
+  <si>
+    <t>operationhoursfile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_other_services</t>
+  </si>
+  <si>
+    <t>branchfloorlevelfile</t>
+  </si>
+  <si>
+    <t>eventtypefile</t>
+  </si>
+  <si>
+    <t>e_b_m_events_rental_costs</t>
+  </si>
+  <si>
+    <t>facilitiesfile</t>
+  </si>
+  <si>
+    <t>e_b_m_locations</t>
+  </si>
+  <si>
+    <t>ingressandegressfile</t>
+  </si>
+  <si>
+    <t>SYSTEM SETUP - ACCOUNTING</t>
+  </si>
+  <si>
+    <t>e_b_m_moa_other_details</t>
+  </si>
+  <si>
+    <t>chargestagfile</t>
+  </si>
+  <si>
+    <t>liabilitiesfile</t>
+  </si>
+  <si>
+    <t>t_m_s_tenant_privileges</t>
+  </si>
+  <si>
+    <t>e_b_m_moa_promotions</t>
+  </si>
+  <si>
+    <t>checkby</t>
+  </si>
+  <si>
+    <t>e_b_m_moa_services</t>
+  </si>
+  <si>
+    <t>logisticsfile</t>
+  </si>
+  <si>
+    <t>e_b_m_notary_details</t>
+  </si>
+  <si>
+    <t>clearancefile</t>
+  </si>
+  <si>
+    <t>moaamendeventschedulefile</t>
+  </si>
+  <si>
+    <t>e_b_m_organizers</t>
+  </si>
+  <si>
+    <t>moaamendmentfile</t>
+  </si>
+  <si>
+    <t>e_b_m_payment_statuses</t>
+  </si>
+  <si>
+    <t>clientofferhistoryfile</t>
+  </si>
+  <si>
+    <t>moaamendparticularsfile</t>
+  </si>
+  <si>
+    <t>LEASING</t>
+  </si>
+  <si>
+    <t>t_m_s_award_notices</t>
+  </si>
+  <si>
+    <t>e_b_m_rental_schemes</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>moaamendperiodcoveredfile</t>
+  </si>
+  <si>
+    <t>t_m_s_contracts</t>
+  </si>
+  <si>
+    <t>e_b_m_transaction_types</t>
+  </si>
+  <si>
+    <t>cmdmextfile</t>
+  </si>
+  <si>
+    <t>moaamendrepresentativefile</t>
+  </si>
+  <si>
+    <t>Sub-table</t>
+  </si>
+  <si>
+    <t>contractrenewalfile</t>
+  </si>
+  <si>
+    <t>failed_jobs</t>
+  </si>
+  <si>
+    <t>cmdmfile</t>
+  </si>
+  <si>
+    <t>moacancellationfile</t>
+  </si>
+  <si>
+    <t>fisher_announcements</t>
+  </si>
+  <si>
     <t>companyaccountfile</t>
-  </si>
-  <si>
-    <t>business_units</t>
-  </si>
-  <si>
-    <t>amendparticularsfile</t>
-  </si>
-  <si>
-    <t>chargesfile</t>
-  </si>
-  <si>
-    <t>t_m_s_tenant_types</t>
-  </si>
-  <si>
-    <t>tenanttypefile</t>
-  </si>
-  <si>
-    <t>companies</t>
-  </si>
-  <si>
-    <t>amendpayschedulefile</t>
-  </si>
-  <si>
-    <t>clausesfile</t>
-  </si>
-  <si>
-    <t>t_m_s_business_categories</t>
-  </si>
-  <si>
-    <t>businesscategoryfile</t>
-  </si>
-  <si>
-    <t>amendrentalchargesfile</t>
-  </si>
-  <si>
-    <t>clientofferfile</t>
-  </si>
-  <si>
-    <t>t_m_s_rental_schemes</t>
-  </si>
-  <si>
-    <t>rentalschemefile</t>
-  </si>
-  <si>
-    <t>e_b_m_authorized_signatories</t>
-  </si>
-  <si>
-    <t>approveby</t>
-  </si>
-  <si>
-    <t>clienttypefile</t>
-  </si>
-  <si>
-    <t>t_m_s_charges</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>e_b_m_billing_terms</t>
-  </si>
-  <si>
-    <t>ar1</t>
-  </si>
-  <si>
-    <t>doctypefile</t>
-  </si>
-  <si>
-    <t>e_b_m_event_types</t>
-  </si>
-  <si>
-    <t>ar2</t>
-  </si>
-  <si>
-    <t>documentfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events</t>
-  </si>
-  <si>
-    <t>at_copy</t>
-  </si>
-  <si>
-    <t>epfdoctypefile</t>
-  </si>
-  <si>
-    <t>SYSTEM SETUP - OPERATION</t>
-  </si>
-  <si>
-    <t>t_m_s_preconstruction_requirements</t>
-  </si>
-  <si>
-    <t>preconstructionfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_amendment</t>
-  </si>
-  <si>
-    <t>epftypefile</t>
-  </si>
-  <si>
-    <t>t_m_s_preoperational_requirements</t>
-  </si>
-  <si>
-    <t>preoperationfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_amendment_information</t>
-  </si>
-  <si>
-    <t>aur_sig</t>
-  </si>
-  <si>
-    <t>eventclassfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_epf_information</t>
-  </si>
-  <si>
-    <t>bank</t>
-  </si>
-  <si>
-    <t>eventfile</t>
-  </si>
-  <si>
-    <t>t_m_s_provisions</t>
-  </si>
-  <si>
-    <t>provisionsfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_ingress_egress</t>
-  </si>
-  <si>
-    <t>bankfile</t>
-  </si>
-  <si>
-    <t>eventperiodcoveredfile</t>
-  </si>
-  <si>
-    <t>t_m_s_meters</t>
-  </si>
-  <si>
-    <t>meterfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_moa_information</t>
-  </si>
-  <si>
-    <t>eventschedulefile</t>
-  </si>
-  <si>
-    <t>t_m_s_operational_hours</t>
-  </si>
-  <si>
-    <t>operationhoursfile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_other_services</t>
-  </si>
-  <si>
-    <t>branchfloorlevelfile</t>
-  </si>
-  <si>
-    <t>eventtypefile</t>
-  </si>
-  <si>
-    <t>e_b_m_events_rental_costs</t>
-  </si>
-  <si>
-    <t>facilitiesfile</t>
-  </si>
-  <si>
-    <t>e_b_m_locations</t>
-  </si>
-  <si>
-    <t>ingressandegressfile</t>
-  </si>
-  <si>
-    <t>SYSTEM SETUP - ACCOUNTING</t>
-  </si>
-  <si>
-    <t>e_b_m_moa_other_details</t>
-  </si>
-  <si>
-    <t>chargestagfile</t>
-  </si>
-  <si>
-    <t>liabilitiesfile</t>
-  </si>
-  <si>
-    <t>t_m_s_tenant_privileges</t>
-  </si>
-  <si>
-    <t>e_b_m_moa_promotions</t>
-  </si>
-  <si>
-    <t>checkby</t>
-  </si>
-  <si>
-    <t>e_b_m_moa_services</t>
-  </si>
-  <si>
-    <t>logisticsfile</t>
-  </si>
-  <si>
-    <t>e_b_m_notary_details</t>
-  </si>
-  <si>
-    <t>clearancefile</t>
-  </si>
-  <si>
-    <t>moaamendeventschedulefile</t>
-  </si>
-  <si>
-    <t>e_b_m_organizers</t>
-  </si>
-  <si>
-    <t>moaamendmentfile</t>
-  </si>
-  <si>
-    <t>e_b_m_payment_statuses</t>
-  </si>
-  <si>
-    <t>clientofferhistoryfile</t>
-  </si>
-  <si>
-    <t>moaamendparticularsfile</t>
-  </si>
-  <si>
-    <t>t_m_s_award_notices</t>
-  </si>
-  <si>
-    <t>e_b_m_rental_schemes</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>moaamendperiodcoveredfile</t>
-  </si>
-  <si>
-    <t>t_m_s_contracts</t>
-  </si>
-  <si>
-    <t>e_b_m_transaction_types</t>
-  </si>
-  <si>
-    <t>cmdmextfile</t>
-  </si>
-  <si>
-    <t>moaamendrepresentativefile</t>
-  </si>
-  <si>
-    <t>Sub-table</t>
-  </si>
-  <si>
-    <t>contractrenewalfile</t>
-  </si>
-  <si>
-    <t>failed_jobs</t>
-  </si>
-  <si>
-    <t>cmdmfile</t>
-  </si>
-  <si>
-    <t>moacancellationfile</t>
-  </si>
-  <si>
-    <t>fisher_announcements</t>
   </si>
   <si>
     <t>moacateringfile</t>
@@ -753,9 +759,6 @@
     <t>modulefile</t>
   </si>
   <si>
-    <t>tenantaccountfile</t>
-  </si>
-  <si>
     <t>t_m_s_meter_type_rates</t>
   </si>
   <si>
@@ -1099,9 +1102,6 @@
   </si>
   <si>
     <t>SYSTEM SETUP - TREASURY</t>
-  </si>
-  <si>
-    <t>LEASING</t>
   </si>
   <si>
     <t>OPERATION</t>
@@ -7280,7 +7280,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7330,6 +7330,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
@@ -7677,48 +7680,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>407035</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133985</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>407035</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>181610</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="20556855" y="324485"/>
-          <a:ext cx="1828800" cy="4048125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -7738,7 +7699,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7747,6 +7708,90 @@
         <a:xfrm>
           <a:off x="22588220" y="4505325"/>
           <a:ext cx="2514600" cy="2276475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>261620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>356870</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20411440" y="425450"/>
+          <a:ext cx="1924050" cy="3819525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20422870" y="4381500"/>
+          <a:ext cx="1257300" cy="1400175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8022,8 +8067,8 @@
   <sheetPr/>
   <dimension ref="A2:M151"/>
   <sheetViews>
-    <sheetView topLeftCell="C88" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55:I62"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -8168,7 +8213,7 @@
       <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -8254,7 +8299,7 @@
       <c r="H11" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="18" t="s">
         <v>50</v>
       </c>
       <c r="J11" t="s">
@@ -8348,7 +8393,7 @@
       <c r="H16" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="18" t="s">
         <v>50</v>
       </c>
       <c r="J16" t="s">
@@ -8443,7 +8488,7 @@
       <c r="H20" t="s">
         <v>61</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="18" t="s">
         <v>50</v>
       </c>
       <c r="J20" t="s">
@@ -8480,7 +8525,7 @@
       <c r="H22" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="18" t="s">
         <v>50</v>
       </c>
       <c r="J22" t="s">
@@ -8568,10 +8613,10 @@
         <v>108</v>
       </c>
       <c r="H28" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="I28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J28" t="s">
         <v>13</v>
@@ -8582,16 +8627,16 @@
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K29" t="s">
         <v>44</v>
@@ -8599,19 +8644,19 @@
     </row>
     <row r="30" spans="2:12">
       <c r="B30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L30" t="s">
         <v>51</v>
@@ -8619,47 +8664,47 @@
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="2:6">
@@ -8667,35 +8712,35 @@
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="2:11">
       <c r="B36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I36" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K36" t="s">
         <v>21</v>
@@ -8703,16 +8748,16 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K37" t="s">
         <v>25</v>
@@ -8720,16 +8765,16 @@
     </row>
     <row r="38" spans="2:11">
       <c r="B38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F38" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K38" t="s">
         <v>28</v>
@@ -8743,10 +8788,10 @@
         <v>57</v>
       </c>
       <c r="F39" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K39" t="s">
         <v>34</v>
@@ -8754,16 +8799,16 @@
     </row>
     <row r="40" spans="2:11">
       <c r="B40" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F40" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I40" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K40" t="s">
         <v>39</v>
@@ -8771,13 +8816,13 @@
     </row>
     <row r="41" spans="2:11">
       <c r="B41" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K41" t="s">
         <v>43</v>
@@ -8785,224 +8830,224 @@
     </row>
     <row r="42" spans="2:6">
       <c r="B42" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F42" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="2:11">
       <c r="B43" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F43" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I43" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K43" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="2:9">
       <c r="B44" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F44" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I44" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="2:9">
       <c r="B45" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F45" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I45" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F46" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F47" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F48" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="2:13">
       <c r="B49" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D49" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H49" t="s">
         <v>61</v>
       </c>
       <c r="I49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K49" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L49" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="2:11">
       <c r="B50" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D50" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F50" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K50" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D51" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F51" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" ht="16" customHeight="1" spans="2:13">
       <c r="B52" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D52" t="s">
         <v>23</v>
       </c>
       <c r="F52" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I52" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K52" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L52" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D53" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F53" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D54" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F54" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="2:11">
       <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" t="s">
+        <v>200</v>
+      </c>
+      <c r="F55" t="s">
+        <v>201</v>
+      </c>
+      <c r="I55" t="s">
+        <v>202</v>
+      </c>
+      <c r="K55" t="s">
         <v>197</v>
-      </c>
-      <c r="D55" t="s">
-        <v>198</v>
-      </c>
-      <c r="F55" t="s">
-        <v>199</v>
-      </c>
-      <c r="I55" t="s">
-        <v>200</v>
-      </c>
-      <c r="K55" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="56" spans="2:11">
       <c r="B56" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D56" t="s">
         <v>80</v>
       </c>
       <c r="F56" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I56" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="K56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="2:11">
@@ -9010,13 +9055,13 @@
         <v>41</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F57" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I57" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K57" t="s">
         <v>80</v>
@@ -9027,16 +9072,16 @@
         <v>50</v>
       </c>
       <c r="D58" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F58" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I58" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="K58" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="2:11">
@@ -9044,136 +9089,136 @@
         <v>31</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F59" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="I59" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K59" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="2:11">
       <c r="B60" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D60" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F60" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I60" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K60" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="2:11">
       <c r="B61" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F61" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I61" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K61" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="2:9">
       <c r="B62" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D62" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F62" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="I62" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="2:6">
       <c r="B63" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D63" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F63" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F64" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F65" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="2:12">
       <c r="B66" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D66" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I66" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K66" t="s">
         <v>94</v>
       </c>
       <c r="L66" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="2:12">
       <c r="B67" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D67" t="s">
         <v>84</v>
       </c>
       <c r="I67" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L67" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="2:12">
       <c r="B68" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D68" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L68" t="s">
         <v>80</v>
@@ -9181,77 +9226,77 @@
     </row>
     <row r="69" spans="2:12">
       <c r="B69" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D69" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L69" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="2:12">
       <c r="B70" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D70" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L70" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="2:12">
       <c r="B71" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D71" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I71" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L71" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="2:12">
       <c r="B72" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I72" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L72" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="2:12">
       <c r="B73" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D73" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I73" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L73" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="2:12">
       <c r="B74" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I74" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L74" t="s">
         <v>46</v>
@@ -9259,26 +9304,26 @@
     </row>
     <row r="75" spans="2:4">
       <c r="B75" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D75" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D76" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="78" spans="2:9">
@@ -9286,59 +9331,59 @@
         <v>79</v>
       </c>
       <c r="D78" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I78" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="79" spans="2:9">
       <c r="B79" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D79" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I79" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="2:9">
       <c r="B80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D80" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I80" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="2:9">
       <c r="B81" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D81" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I81" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D82" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D83" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -9346,23 +9391,23 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:9">
       <c r="B85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D85" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I85" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D86" t="s">
         <v>63</v>
@@ -9370,7 +9415,7 @@
     </row>
     <row r="87" spans="2:4">
       <c r="B87" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D87" t="s">
         <v>67</v>
@@ -9378,10 +9423,10 @@
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D88" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -9389,7 +9434,7 @@
         <v>62</v>
       </c>
       <c r="D89" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="2:9">
@@ -9400,7 +9445,7 @@
         <v>75</v>
       </c>
       <c r="I90" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -9408,15 +9453,15 @@
         <v>74</v>
       </c>
       <c r="D91" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D92" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -9424,48 +9469,48 @@
         <v>45</v>
       </c>
       <c r="D93" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="94" spans="2:12">
       <c r="B94" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D94" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I94" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L94" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="2:9">
       <c r="B95" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D95" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="I95" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="2:9">
       <c r="B96" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D96" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I96" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="2:4">
       <c r="B97" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D97" t="s">
         <v>46</v>
@@ -9473,48 +9518,48 @@
     </row>
     <row r="98" spans="2:4">
       <c r="B98" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D98" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D99" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="2:12">
       <c r="B100" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D100" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I100" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L100" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D101" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D102" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="103" spans="2:4">
@@ -9522,95 +9567,95 @@
         <v>96</v>
       </c>
       <c r="D103" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D104" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="B105" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D105" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D106" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="2:4">
       <c r="B107" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D107" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="B108" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D108" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="109" spans="2:4">
       <c r="B109" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D109" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D110" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="B111" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D111" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="B112" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D112" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="B113" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D113" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="114" spans="2:4">
       <c r="B114" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D114" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="115" spans="2:4">
@@ -9618,25 +9663,25 @@
         <v>36</v>
       </c>
       <c r="D115" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="B116" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D116" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="4:4">
       <c r="D117" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="118" spans="4:4">
       <c r="D118" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" spans="4:4">
@@ -9646,162 +9691,162 @@
     </row>
     <row r="120" spans="4:4">
       <c r="D120" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="121" spans="4:4">
       <c r="D121" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="122" spans="4:4">
       <c r="D122" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="123" spans="4:4">
       <c r="D123" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="124" spans="4:4">
       <c r="D124" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="125" spans="4:4">
       <c r="D125" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="126" spans="4:4">
       <c r="D126" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="127" spans="4:4">
       <c r="D127" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" spans="4:4">
       <c r="D128" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="129" spans="4:4">
       <c r="D129" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="130" spans="4:4">
       <c r="D130" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="4:4">
       <c r="D131" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="132" spans="4:4">
       <c r="D132" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="4:4">
       <c r="D133" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="134" spans="4:4">
       <c r="D134" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="135" spans="4:4">
       <c r="D135" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="136" spans="4:4">
       <c r="D136" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="137" spans="4:4">
       <c r="D137" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="138" spans="4:4">
       <c r="D138" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="139" spans="4:4">
       <c r="D139" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="140" spans="4:4">
       <c r="D140" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="141" spans="4:4">
       <c r="D141" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="4:4">
       <c r="D142" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="143" spans="4:4">
       <c r="D143" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="144" spans="4:4">
       <c r="D144" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="145" spans="4:4">
       <c r="D145" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="146" spans="4:4">
       <c r="D146" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="147" spans="4:4">
       <c r="D147" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="148" spans="4:4">
       <c r="D148" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" spans="4:4">
       <c r="D149" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="150" spans="4:4">
       <c r="D150" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="151" spans="4:4">
       <c r="D151" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -9878,7 +9923,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -9898,17 +9943,17 @@
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>337</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="3:3">
@@ -9937,10 +9982,10 @@
   <sheetPr/>
   <dimension ref="B1:DT37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="CH1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H1:H8"/>
+      <selection pane="bottomLeft" activeCell="CN1" sqref="CN1:CN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15"/>
@@ -10150,19 +10195,19 @@
         <v>106</v>
       </c>
       <c r="AB1" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AD1" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AE1" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AF1" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AG1" s="10" t="s">
         <v>22</v>
@@ -10171,67 +10216,67 @@
         <v>18</v>
       </c>
       <c r="AI1" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ1" s="10" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AK1" s="10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AL1" s="10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM1" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AN1" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AO1" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AP1" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AQ1" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AR1" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AS1" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AT1" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AU1" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AV1" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AW1" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AX1" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AY1" s="10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AZ1" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="BA1" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BB1" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="BC1" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="BD1" s="10" t="s">
         <v>41</v>
@@ -10243,91 +10288,91 @@
         <v>31</v>
       </c>
       <c r="BG1" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="BI1" s="10" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="BJ1" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="BK1" s="10" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="BL1" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="BM1" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="BN1" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="BO1" s="10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="BP1" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="BQ1" s="10" t="s">
         <v>79</v>
       </c>
       <c r="BR1" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="BS1" s="10" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="BT1" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="BU1" s="10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="BV1" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="BW1" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="BX1" s="10" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="BY1" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="BZ1" s="10" t="s">
         <v>83</v>
       </c>
       <c r="CA1" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="CB1" s="10" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="CC1" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="CD1" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="CE1" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="CF1" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="CD1" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="CE1" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="CF1" s="10" t="s">
-        <v>250</v>
-      </c>
       <c r="CG1" s="10" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="CH1" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="CI1" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="CI1" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="CJ1" s="10" t="s">
         <v>62</v>
@@ -10339,79 +10384,79 @@
         <v>74</v>
       </c>
       <c r="CM1" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="CN1" s="10" t="s">
         <v>45</v>
       </c>
       <c r="CO1" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="CP1" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="CQ1" s="10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="CR1" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="CS1" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="CT1" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="CS1" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="CT1" s="10" t="s">
-        <v>274</v>
-      </c>
       <c r="CU1" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="CV1" s="10" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="CW1" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="CX1" s="10" t="s">
         <v>96</v>
       </c>
       <c r="CY1" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="CZ1" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="DA1" s="10" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="DB1" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="DC1" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="DD1" s="10" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="DE1" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="DF1" s="10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="DG1" s="10" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="DH1" s="10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="DI1" s="10" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="DJ1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="DK1" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="DL1" s="10" t="s">
         <v>341</v>
@@ -15207,10 +15252,10 @@
   <sheetPr/>
   <dimension ref="B2:ET2922"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="U1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="CH1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AE9" sqref="AE2:AE9"/>
+      <selection pane="bottomLeft" activeCell="CR2" sqref="CR2:CR9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -15438,175 +15483,175 @@
         <v>107</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AG2" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AH2" s="10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AI2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="AJ2" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AL2" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AM2" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AN2" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AO2" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AP2" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AQ2" s="10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AR2" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AS2" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AT2" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AU2" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AV2" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AW2" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AX2" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AY2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="AZ2" s="10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="BA2" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="BB2" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="BC2" s="10" t="s">
         <v>80</v>
       </c>
       <c r="BD2" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="BE2" s="10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="BF2" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="BG2" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="BH2" s="10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="BI2" s="10" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="BJ2" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="BK2" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="BL2" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="BM2" s="10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="BN2" s="10" t="s">
         <v>84</v>
       </c>
       <c r="BO2" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BP2" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="BQ2" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="BR2" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="BS2" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="BT2" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="BU2" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="BV2" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="BW2" s="10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="BX2" s="10" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="BY2" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="BZ2" s="10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="CA2" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="CB2" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="CC2" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="CD2" s="10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CE2" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="CF2" s="10" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="CG2" s="10" t="s">
         <v>63</v>
@@ -15615,196 +15660,196 @@
         <v>67</v>
       </c>
       <c r="CI2" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="CJ2" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="CK2" s="10" t="s">
         <v>75</v>
       </c>
       <c r="CL2" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="CM2" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="CN2" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="CO2" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="CP2" s="10" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="CQ2" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="CR2" s="10" t="s">
         <v>46</v>
       </c>
       <c r="CS2" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="CT2" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="CU2" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="CV2" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="CW2" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="CX2" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="CY2" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="CZ2" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="DA2" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="DB2" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="DC2" s="10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="DD2" s="10" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="DE2" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="DF2" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="DG2" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="DH2" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="DI2" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="DJ2" s="10" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="DK2" s="10" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="DL2" s="10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="DM2" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="DN2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="DO2" s="10" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="DP2" s="10" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="DQ2" s="10" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="DR2" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="DS2" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="DT2" s="10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="DU2" s="10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="DV2" s="10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="DW2" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="DX2" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="DY2" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="DZ2" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="EA2" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="EB2" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="EC2" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="ED2" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="EE2" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="EF2" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="EG2" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="EH2" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="DZ2" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="EA2" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="EB2" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="EC2" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="ED2" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="EE2" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="EF2" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="EG2" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="EH2" s="10" t="s">
-        <v>317</v>
-      </c>
       <c r="EI2" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="EJ2" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="EK2" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="EL2" s="10" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="EM2" s="10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="EN2" s="10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="EO2" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="EP2" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="EQ2" s="10" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="ER2" s="10" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="ES2" s="10" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="ET2" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="2:150">
@@ -18936,7 +18981,7 @@
       </c>
       <c r="CA10" s="5"/>
       <c r="CB10" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="CC10" s="5"/>
       <c r="CD10" s="5"/>
@@ -19861,7 +19906,7 @@
       <c r="BJ13" s="5"/>
       <c r="BK13" s="5"/>
       <c r="BL13" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="BM13" s="5"/>
       <c r="BN13" s="5" t="s">
@@ -20154,7 +20199,7 @@
       <c r="BJ14" s="5"/>
       <c r="BK14" s="5"/>
       <c r="BL14" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="BM14" s="5"/>
       <c r="BN14" s="5" t="s">
@@ -20190,7 +20235,7 @@
       </c>
       <c r="CA14" s="5"/>
       <c r="CB14" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="CC14" s="5"/>
       <c r="CD14" s="5"/>
@@ -21966,7 +22011,7 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>1543</v>
@@ -22575,7 +22620,7 @@
         <v>896</v>
       </c>
       <c r="BR23" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="BS23" s="5"/>
       <c r="BT23" s="5" t="s">
@@ -22638,7 +22683,7 @@
       <c r="DC23" s="5"/>
       <c r="DD23" s="5"/>
       <c r="DE23" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="DF23" s="5"/>
       <c r="DG23" s="5"/>
@@ -23084,7 +23129,7 @@
         <v>1608</v>
       </c>
       <c r="CM25" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="CN25" s="5"/>
       <c r="CO25" s="5"/>
@@ -23898,7 +23943,7 @@
       <c r="AE29" s="5"/>
       <c r="AF29" s="5"/>
       <c r="AG29" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AH29" s="5"/>
       <c r="AI29" s="5"/>
@@ -24729,7 +24774,7 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
       <c r="Z33" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AA33" s="5" t="s">
         <v>945</v>
@@ -24949,7 +24994,7 @@
       <c r="AK34" s="5"/>
       <c r="AL34" s="5"/>
       <c r="AM34" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AN34" s="5"/>
       <c r="AO34" s="5"/>
@@ -25148,7 +25193,7 @@
       <c r="AK35" s="5"/>
       <c r="AL35" s="5"/>
       <c r="AM35" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN35" s="5"/>
       <c r="AO35" s="5"/>
@@ -25175,7 +25220,7 @@
       <c r="BF35" s="5"/>
       <c r="BG35" s="5"/>
       <c r="BH35" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="BI35" s="5"/>
       <c r="BJ35" s="5"/>
@@ -34824,7 +34869,7 @@
         <v>1803</v>
       </c>
       <c r="AA93" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AB93" s="5"/>
       <c r="AC93" s="5"/>
@@ -43491,7 +43536,7 @@
     </row>
     <row r="478" spans="2:2">
       <c r="B478" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="479" spans="2:2">
@@ -44471,7 +44516,7 @@
     </row>
     <row r="675" spans="2:2">
       <c r="B675" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="676" spans="2:2">
@@ -45066,7 +45111,7 @@
     </row>
     <row r="800" spans="2:2">
       <c r="B800" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="801" spans="2:2">
@@ -45886,12 +45931,12 @@
     </row>
     <row r="970" spans="2:2">
       <c r="B970" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="971" spans="2:2">
       <c r="B971" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="972" spans="2:2">
@@ -47866,7 +47911,7 @@
     </row>
     <row r="1387" spans="2:2">
       <c r="B1387" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1388" spans="2:2">
@@ -48131,12 +48176,12 @@
     </row>
     <row r="1444" spans="2:2">
       <c r="B1444" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="1445" spans="2:2">
       <c r="B1445" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1446" spans="2:2">
@@ -48796,7 +48841,7 @@
     </row>
     <row r="1583" spans="2:2">
       <c r="B1583" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="1584" spans="2:2">
@@ -49961,7 +50006,7 @@
     </row>
     <row r="1826" spans="2:2">
       <c r="B1826" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="1827" spans="2:2">
@@ -49981,7 +50026,7 @@
     </row>
     <row r="1830" spans="2:2">
       <c r="B1830" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1831" spans="2:2">
@@ -50576,7 +50621,7 @@
     </row>
     <row r="1960" spans="2:2">
       <c r="B1960" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1961" spans="2:2">
@@ -52271,7 +52316,7 @@
     </row>
     <row r="2317" spans="2:2">
       <c r="B2317" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2318" spans="2:2">
@@ -55261,115 +55306,115 @@
         <v>108</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AG2" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AH2" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AI2" s="10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AJ2" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AL2" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AM2" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AN2" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AO2" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AP2" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AQ2" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AR2" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AS2" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AT2" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AU2" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AV2" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AW2" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AX2" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AY2" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AZ2" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="BA2" s="10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="BB2" s="10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="BC2" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="BD2" s="10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="BE2" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="BF2" s="10" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="BG2" s="10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="BH2" s="10" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="BI2" s="10" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="BJ2" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="BK2" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="BL2" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:64">
@@ -57233,7 +57278,7 @@
       <c r="AP18" s="5"/>
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
@@ -58587,7 +58632,7 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
@@ -59183,7 +59228,7 @@
       <c r="AF44" s="5"/>
       <c r="AG44" s="5"/>
       <c r="AH44" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AI44" s="5"/>
       <c r="AJ44" s="5"/>
@@ -59667,7 +59712,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
@@ -60057,7 +60102,7 @@
       <c r="AV56" s="5"/>
       <c r="AW56" s="5"/>
       <c r="AX56" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AY56" s="5"/>
       <c r="AZ56" s="5"/>
@@ -60721,7 +60766,7 @@
       <c r="AF66" s="5"/>
       <c r="AG66" s="5"/>
       <c r="AH66" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AI66" s="5"/>
       <c r="AJ66" s="5"/>
@@ -60901,10 +60946,10 @@
   <sheetPr/>
   <dimension ref="A1:N463"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D361" sqref="D361"/>
+      <selection pane="bottomLeft" activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -61330,7 +61375,7 @@
         <v>31</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>2101</v>
@@ -61886,7 +61931,7 @@
         <v>345</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="139" spans="2:3">
@@ -62032,7 +62077,7 @@
     </row>
     <row r="159" spans="2:3">
       <c r="B159" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>44</v>
@@ -62376,7 +62421,7 @@
         <v>436</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="185" spans="2:6">
@@ -62434,7 +62479,7 @@
     </row>
     <row r="192" spans="2:3">
       <c r="B192" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>1349</v>
@@ -62970,7 +63015,7 @@
     </row>
     <row r="265" spans="3:3">
       <c r="C265" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="266" spans="3:3">
@@ -63125,16 +63170,16 @@
     </row>
     <row r="299" spans="2:14">
       <c r="B299" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C299" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="M299" s="3" t="s">
         <v>2106</v>
       </c>
       <c r="N299" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="300" customHeight="1" spans="2:13">
@@ -63342,7 +63387,7 @@
     </row>
     <row r="327" spans="3:3">
       <c r="C327" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="328" spans="3:3">
@@ -63463,7 +63508,7 @@
       <c r="F348" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="G348" s="14" t="s">
+      <c r="G348" s="6" t="s">
         <v>2107</v>
       </c>
     </row>
@@ -63491,7 +63536,7 @@
         <v>38</v>
       </c>
       <c r="C352" s="10" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
     </row>
     <row r="353" spans="2:7">
@@ -63555,7 +63600,7 @@
       <c r="F357" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="G357" s="14" t="s">
+      <c r="G357" s="6" t="s">
         <v>2107</v>
       </c>
     </row>
@@ -63582,7 +63627,296 @@
       </c>
       <c r="F359" s="5"/>
     </row>
-    <row r="368" ht="16" customHeight="1"/>
+    <row r="364" spans="2:3">
+      <c r="B364" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C364" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="365" spans="2:6">
+      <c r="B365" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C365" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F365" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="366" spans="2:6">
+      <c r="B366" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C366" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="F366" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="367" spans="2:6">
+      <c r="B367" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C367" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="F367" s="5"/>
+    </row>
+    <row r="368" ht="16" customHeight="1" spans="2:7">
+      <c r="B368" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C368" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="F368" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="G368" s="5" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="369" spans="2:7">
+      <c r="B369" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C369" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F369" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G369" s="5" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="370" spans="2:7">
+      <c r="B370" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C370" s="5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F370" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="G370" s="5" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="371" spans="2:6">
+      <c r="B371" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C371" s="5" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F371" s="5"/>
+    </row>
+    <row r="372" spans="2:6">
+      <c r="B372" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C372" s="5" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F372" s="5"/>
+    </row>
+    <row r="373" spans="2:6">
+      <c r="B373" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C373" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F373" s="5"/>
+    </row>
+    <row r="378" spans="2:3">
+      <c r="B378" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C378" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="379" spans="2:7">
+      <c r="B379" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C379" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F379" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G379" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="380" spans="2:6">
+      <c r="B380" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>875</v>
+      </c>
+      <c r="F380" s="5"/>
+    </row>
+    <row r="381" spans="2:7">
+      <c r="B381" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C381" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="F381" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="G381" s="5" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="382" spans="2:7">
+      <c r="B382" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="383" spans="2:6">
+      <c r="B383" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="F383" s="5"/>
+    </row>
+    <row r="384" ht="60" spans="2:7">
+      <c r="B384" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="F384" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G384" s="4" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="385" spans="2:6">
+      <c r="B385" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="F385" s="5"/>
+    </row>
+    <row r="386" spans="2:6">
+      <c r="B386" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="F386" s="5"/>
+    </row>
+    <row r="389" spans="2:3">
+      <c r="B389" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C389" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="390" spans="2:6">
+      <c r="B390" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F390" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="391" spans="2:6">
+      <c r="B391" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C391" s="5" t="s">
+        <v>914</v>
+      </c>
+      <c r="F391" s="5"/>
+    </row>
+    <row r="392" spans="2:7">
+      <c r="B392" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="F392" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="393" spans="2:6">
+      <c r="B393" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C393" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F393" s="5"/>
+    </row>
+    <row r="394" spans="2:7">
+      <c r="B394" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F394" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G394" s="5" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="395" ht="60" spans="2:7">
+      <c r="B395" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C395" s="5" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F395" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G395" s="14" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="396" spans="2:6">
+      <c r="B396" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C396" s="5" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F396" s="5"/>
+    </row>
+    <row r="397" spans="2:6">
+      <c r="B397" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="F397" s="5"/>
+    </row>
     <row r="413" ht="17" customHeight="1"/>
     <row r="431" ht="17" customHeight="1"/>
     <row r="446" ht="18" customHeight="1"/>
@@ -63601,7 +63935,7 @@
   <sheetPr/>
   <dimension ref="B1:H336"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A165" workbookViewId="0">
       <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
@@ -63635,16 +63969,16 @@
     </row>
     <row r="2" customHeight="1" spans="2:7">
       <c r="B2" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="2:7">
@@ -63891,10 +64225,10 @@
         <v>2113</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G31" t="s">
         <v>1680</v>
@@ -64004,7 +64338,7 @@
     </row>
     <row r="44" customHeight="1" spans="2:7">
       <c r="B44" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C44" t="s">
         <v>2115</v>
@@ -64118,7 +64452,7 @@
     </row>
     <row r="59" customHeight="1" spans="2:7">
       <c r="B59" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>67</v>
@@ -64278,16 +64612,16 @@
     <row r="75" customHeight="1"/>
     <row r="76" customHeight="1" spans="2:6">
       <c r="B76" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>2118</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" customHeight="1" spans="2:6">
@@ -64461,16 +64795,16 @@
     </row>
     <row r="97" customHeight="1" spans="2:7">
       <c r="B97" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>2119</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G97" t="s">
         <v>891</v>
@@ -64632,16 +64966,16 @@
     </row>
     <row r="115" customHeight="1" spans="2:6">
       <c r="B115" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>2120</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" customHeight="1" spans="2:6">
@@ -64728,7 +65062,7 @@
         <v>634</v>
       </c>
       <c r="C124" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F124" t="s">
         <v>971</v>
@@ -64739,7 +65073,7 @@
         <v>567</v>
       </c>
       <c r="C125" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F125" t="s">
         <v>1260</v>
@@ -64784,7 +65118,7 @@
     <row r="131" customHeight="1"/>
     <row r="132" customHeight="1" spans="2:6">
       <c r="B132" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>94</v>
@@ -64919,13 +65253,13 @@
     <row r="149" customHeight="1"/>
     <row r="150" customHeight="1" spans="2:6">
       <c r="B150" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" customHeight="1" spans="2:6">
@@ -65130,12 +65464,12 @@
     </row>
     <row r="182" customHeight="1" spans="6:6">
       <c r="F182" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="183" customHeight="1" spans="6:6">
       <c r="F183" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" customHeight="1" spans="6:6">
@@ -65153,13 +65487,13 @@
     <row r="188" customHeight="1"/>
     <row r="189" customHeight="1" spans="2:6">
       <c r="B189" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="190" customHeight="1" spans="2:6">
@@ -65259,13 +65593,13 @@
     </row>
     <row r="200" customHeight="1" spans="2:6">
       <c r="B200" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F200" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="201" customHeight="1" spans="2:6">
@@ -65276,7 +65610,7 @@
         <v>349</v>
       </c>
       <c r="F201" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="202" customHeight="1" spans="2:6">
@@ -65348,10 +65682,10 @@
     </row>
     <row r="210" customHeight="1" spans="2:6">
       <c r="B210" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F210" t="s">
         <v>1156</v>
@@ -65445,10 +65779,10 @@
     </row>
     <row r="221" customHeight="1" spans="2:6">
       <c r="B221" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F221" t="s">
         <v>1707</v>
@@ -65578,13 +65912,13 @@
     <row r="240" customHeight="1"/>
     <row r="241" customHeight="1" spans="2:6">
       <c r="B241" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="242" customHeight="1" spans="2:6">
@@ -65764,13 +66098,13 @@
     <row r="264" customHeight="1"/>
     <row r="265" customHeight="1" spans="2:6">
       <c r="B265" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C265" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C265" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="F265" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="266" customHeight="1" spans="2:6">
@@ -65896,10 +66230,10 @@
     </row>
     <row r="280" customHeight="1" spans="2:6">
       <c r="B280" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F280" t="s">
         <v>551</v>
@@ -66028,10 +66362,10 @@
     </row>
     <row r="295" customHeight="1" spans="2:6">
       <c r="B295" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F295" t="s">
         <v>1485</v>
@@ -66142,10 +66476,10 @@
     </row>
     <row r="310" spans="2:3">
       <c r="B310" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="311" spans="2:3">
@@ -66223,10 +66557,10 @@
     </row>
     <row r="325" spans="2:3">
       <c r="B325" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="326" spans="2:3">

</xml_diff>